<commit_message>
Add Tests to TP Clients + sistemati test censimento e modifica PG
</commit_message>
<xml_diff>
--- a/docs/tp/Clients.xlsx
+++ b/docs/tp/Clients.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TA\matrix-web-fe-tests\docs\tp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TA\matrix-web-fe-tests\docs\tp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923EC6FE-018D-43EC-AD59-F466D5B19BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FDF69F-AEFE-4444-B486-22FB0269109A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="810" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{BE46A6EB-3E52-4087-BE1D-BF4A8643FA88}"/>
+    <workbookView xWindow="-60" yWindow="-60" windowWidth="28920" windowHeight="15900" xr2:uid="{BE46A6EB-3E52-4087-BE1D-BF4A8643FA88}"/>
   </bookViews>
   <sheets>
     <sheet name="Bobo" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="172">
   <si>
     <t>Oboe Andrea (Leased Employee)</t>
   </si>
@@ -441,6 +441,117 @@
   </si>
   <si>
     <t xml:space="preserve">Verificare che il contatto PEC sia stato inserito correttamente nella tabella del tab Contatti </t>
+  </si>
+  <si>
+    <t>MW : Carta Identità (1)</t>
+  </si>
+  <si>
+    <t>Ricerca di un cliente random senza CI</t>
+  </si>
+  <si>
+    <t>Verificare che l'operazione vada  a buon fine</t>
+  </si>
+  <si>
+    <t>MW : Patente (1)</t>
+  </si>
+  <si>
+    <t>MW : Passaporto (1)</t>
+  </si>
+  <si>
+    <t>MW : Porto D'Armi (1)</t>
+  </si>
+  <si>
+    <t>MW : Tessera Postale (1)</t>
+  </si>
+  <si>
+    <t>MW : Altro Documento (1)</t>
+  </si>
+  <si>
+    <t>Ricerca di un cliente random senza Patente</t>
+  </si>
+  <si>
+    <t>Ricerca di un cliente random senza Passaporto</t>
+  </si>
+  <si>
+    <t>Ricerca di un cliente random senza Porto D'Armi</t>
+  </si>
+  <si>
+    <t>Ricerca di un cliente random senza Tessera Postale</t>
+  </si>
+  <si>
+    <t>Ricerca di un cliente random senza Altro Tipo di Documento</t>
+  </si>
+  <si>
+    <t>Inserire la CI</t>
+  </si>
+  <si>
+    <t>Inserire la Patente</t>
+  </si>
+  <si>
+    <t>Inserire il Passaporto</t>
+  </si>
+  <si>
+    <t>Inserire il Porto D'Armi</t>
+  </si>
+  <si>
+    <t>Inserire la Tessera Postale</t>
+  </si>
+  <si>
+    <t>Inserire tipo di documento Altro</t>
+  </si>
+  <si>
+    <t>MW : Carta Identità (2)</t>
+  </si>
+  <si>
+    <t>MW : Patente (2)</t>
+  </si>
+  <si>
+    <t>MW : Passaporto (2)</t>
+  </si>
+  <si>
+    <t>MW : Porto D'Armi (2)</t>
+  </si>
+  <si>
+    <t>MW : Tessera Postale (2)</t>
+  </si>
+  <si>
+    <t>MW : Altro Documento (2)</t>
+  </si>
+  <si>
+    <t>MW : Carta Identità (3)</t>
+  </si>
+  <si>
+    <t>Verificare la CI inserita</t>
+  </si>
+  <si>
+    <t>MW : Patente (3)</t>
+  </si>
+  <si>
+    <t>Verificare la Patente inserita</t>
+  </si>
+  <si>
+    <t>MW : Passaporto (3)</t>
+  </si>
+  <si>
+    <t>Verificare il Passaporto inserito</t>
+  </si>
+  <si>
+    <t>Verificare il Porto D'Armi inserito</t>
+  </si>
+  <si>
+    <t>Verificare la Tessera Postale inserita</t>
+  </si>
+  <si>
+    <t>MW : Tessera Postale (3)</t>
+  </si>
+  <si>
+    <t>MW : Porto D'Armi (3)</t>
+  </si>
+  <si>
+    <t>MW : Altro Documento (3)</t>
+  </si>
+  <si>
+    <t>Verificare Altro tipo di docmento inserito</t>
   </si>
 </sst>
 </file>
@@ -924,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1AEFEBA-728D-4FDD-9B3D-F6BE0E3793BC}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I39" sqref="A22:I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1552,8 +1663,528 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C33" s="6"/>
+    <row r="22" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I27" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I28" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I31" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I32" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I34" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="K34" s="6"/>
+    </row>
+    <row r="35" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I35" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G36" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I36" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G37" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H37" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I37" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G38" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I38" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G39" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H39" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I39" s="13" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1565,8 +2196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10A60FA2-5DE8-44B4-9E60-8DD49A8388E4}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update clients e legami
</commit_message>
<xml_diff>
--- a/docs/tp/Clients.xlsx
+++ b/docs/tp/Clients.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TA\matrix-web-fe-tests\docs\tp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6F7640-C911-4EFF-9E48-C11290481BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3C8F5F-802B-4BA7-B3BC-7A266319E7E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="810" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{BE46A6EB-3E52-4087-BE1D-BF4A8643FA88}"/>
+    <workbookView xWindow="-19320" yWindow="660" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{BE46A6EB-3E52-4087-BE1D-BF4A8643FA88}"/>
   </bookViews>
   <sheets>
     <sheet name="Bobo" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1179" uniqueCount="261">
   <si>
     <t>Oboe Andrea (Leased Employee)</t>
   </si>
@@ -773,6 +773,62 @@
   </si>
   <si>
     <t>Verifica presenza di tutti i campi titoli -&gt; Documento Principale</t>
+  </si>
+  <si>
+    <t>Clients &gt; Gestione Gruppi Legami &gt; Gestione Gruppi Aziendali</t>
+  </si>
+  <si>
+    <t>MW &gt; Accedere come Delegato Assicurativo di un'agenzia  a piacere &gt; Trovare un cliente persona giuridica &gt; Dettaglio anagrafica &gt; Legami &gt; Procedere con la creazione di un Gruppo aziendale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verificare che l'operazione vada a buon fine e che si apra la maschera per inserire eventuali aderenti </t>
+  </si>
+  <si>
+    <t>Cliccare sul pulsante Inserisci membro&gt; Ricerca &gt; Utilizzare un'anagrafica a piacere già presenti</t>
+  </si>
+  <si>
+    <t>Effettuare l'eliminazione di un solo Appartenente</t>
+  </si>
+  <si>
+    <t>Verificare che l'operazione vada a buon fine e NON sia più presente l'Appartenente eliminato dal gruppo anche accedendo alla CV degli altri Appartenenti e del Capo gruppo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clients &gt; Gestione Gruppi Legami &gt; Gestione Gruppi Aziendali  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verificare che:
+- si apra la ricerca tramite denominazione e funzioni correttamente;
+- NON sia possibile inserire la stessa anagrafica del Capo gruppo anche come Appartenente;
+- sia possibile inserire anagrafiche con un altra sede;
+- NON sia possibile inserire persone fisiche;
+- l'inserimento del Gruppo, Capo gruppo ed Appartenenti vadano a buon fine ed i dati visualizzati nel Dettaglio anagrafica siano corretti;
+- sia riportato qual è il Capo gruppo e quale l'Appartenente;
+- nella sidebar (sotto la denominazione del cliente) NON sia riportato nessun riferimento al Gruppo aziendale;
+</t>
+  </si>
+  <si>
+    <t>MW &gt; Accedere come Delegato Assicurativo di un'agenzia a piacere &gt; Trovare un cliente persona giuridica &gt; Dettaglio anagrafica &gt; Legami &gt; Procedere con la creazione di un Gruppo aziendale &gt; Cliccare sul pulsante Aggiungi nuovo cliente in modo da inserire un nuovo Appartenente &gt; Scegliere un'anagrafica che faccia parte già di un Gruppo aziendale in altra agenzia al di fuori dell'HUB</t>
+  </si>
+  <si>
+    <t>Verificare che si venga bloccati perché l'anagrafica risulta già legata ad un altro Gruppo aziendale (anche se in altra agenzia non dello stesso HUB)</t>
+  </si>
+  <si>
+    <t>MW &gt; Accedere come Delegato Assicurativo di un'agenzia  a piacere &gt; Trovare un cliente persona giuridica &gt; Dettaglio anagrafica &gt; Legami &gt; Procedere con l'eliminazione del gruppo aziendale</t>
+  </si>
+  <si>
+    <t>Verificare che l'operazione di elimina gruppo vada a buon fine</t>
+  </si>
+  <si>
+    <t>MW &gt; Accedere come Fonte Secondaria che NON abbia il permesso applicativo della gestione legami</t>
+  </si>
+  <si>
+    <t>Verificare che NON sia possibile ne modificare ne eliminare i Gruppi aziendali, ma che siano correttamente visibili.</t>
+  </si>
+  <si>
+    <t>Verificare NON sia possibile inserire anagrafiche già assegnate ad un altro Gruppo aziendale (indifferentemente se come Capo gruppo o Appartenente);</t>
+  </si>
+  <si>
+    <t>Verificare NON sia possibile legare più di 3 anagrafiche al gruppo e il messaggio di blocco sia corretto</t>
   </si>
 </sst>
 </file>
@@ -812,7 +868,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -891,8 +947,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -915,12 +977,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -973,10 +1049,20 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
     <cellStyle name="Normale 3" xfId="1" xr:uid="{7717704E-76BB-44C2-A869-36A16CD05F21}"/>
+    <cellStyle name="Normale 4" xfId="2" xr:uid="{849AE8CC-E66E-4DA8-A862-D7F003212C4A}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3253,10 +3339,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10A60FA2-5DE8-44B4-9E60-8DD49A8388E4}">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4954,6 +5040,238 @@
         <v>3</v>
       </c>
     </row>
+    <row r="59" spans="1:9" ht="73.5" x14ac:dyDescent="0.25">
+      <c r="A59" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="B59" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C59" s="21" t="s">
+        <v>247</v>
+      </c>
+      <c r="D59" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="E59" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F59" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G59" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H59" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="I59" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="178.5" x14ac:dyDescent="0.25">
+      <c r="A60" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="B60" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="C60" s="21" t="s">
+        <v>252</v>
+      </c>
+      <c r="D60" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="E60" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F60" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G60" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H60" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="I60" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="42" x14ac:dyDescent="0.25">
+      <c r="A61" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="B61" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="C61" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="D61" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="E61" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F61" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G61" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H61" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="I61" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="42" x14ac:dyDescent="0.25">
+      <c r="A62" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="B62" s="22" t="s">
+        <v>249</v>
+      </c>
+      <c r="C62" s="21" t="s">
+        <v>250</v>
+      </c>
+      <c r="D62" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="E62" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F62" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G62" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H62" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="I62" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="126" x14ac:dyDescent="0.25">
+      <c r="A63" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="B63" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="C63" s="21" t="s">
+        <v>254</v>
+      </c>
+      <c r="D63" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="E63" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F63" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G63" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H63" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="I63" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="42" x14ac:dyDescent="0.25">
+      <c r="A64" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="B64" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="C64" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="D64" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="E64" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F64" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G64" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H64" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="I64" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="73.5" x14ac:dyDescent="0.25">
+      <c r="A65" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="B65" s="21" t="s">
+        <v>255</v>
+      </c>
+      <c r="C65" s="21" t="s">
+        <v>256</v>
+      </c>
+      <c r="D65" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="E65" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F65" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G65" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H65" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="I65" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="42" x14ac:dyDescent="0.25">
+      <c r="A66" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="B66" s="21" t="s">
+        <v>257</v>
+      </c>
+      <c r="C66" s="21" t="s">
+        <v>258</v>
+      </c>
+      <c r="D66" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="E66" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F66" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G66" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H66" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="I66" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated test plan Note di Contratto
</commit_message>
<xml_diff>
--- a/docs/tp/Clients.xlsx
+++ b/docs/tp/Clients.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TA\matrix-web-fe-tests\docs\tp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3C8F5F-802B-4BA7-B3BC-7A266319E7E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC24956-C06B-4F96-8957-38DAAD1CBE4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="660" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{BE46A6EB-3E52-4087-BE1D-BF4A8643FA88}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{BE46A6EB-3E52-4087-BE1D-BF4A8643FA88}"/>
   </bookViews>
   <sheets>
     <sheet name="Bobo" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1179" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="300">
   <si>
     <t>Oboe Andrea (Leased Employee)</t>
   </si>
@@ -775,9 +775,6 @@
     <t>Verifica presenza di tutti i campi titoli -&gt; Documento Principale</t>
   </si>
   <si>
-    <t>Clients &gt; Gestione Gruppi Legami &gt; Gestione Gruppi Aziendali</t>
-  </si>
-  <si>
     <t>MW &gt; Accedere come Delegato Assicurativo di un'agenzia  a piacere &gt; Trovare un cliente persona giuridica &gt; Dettaglio anagrafica &gt; Legami &gt; Procedere con la creazione di un Gruppo aziendale</t>
   </si>
   <si>
@@ -791,9 +788,6 @@
   </si>
   <si>
     <t>Verificare che l'operazione vada a buon fine e NON sia più presente l'Appartenente eliminato dal gruppo anche accedendo alla CV degli altri Appartenenti e del Capo gruppo.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clients &gt; Gestione Gruppi Legami &gt; Gestione Gruppi Aziendali  </t>
   </si>
   <si>
     <t xml:space="preserve">Verificare che:
@@ -829,6 +823,129 @@
   </si>
   <si>
     <t>Verificare NON sia possibile legare più di 3 anagrafiche al gruppo e il messaggio di blocco sia corretto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inserire Titolo e Testo a piacere e cliccare su Salva                                                                   - Verificare che l'operazione vada a buon fine e si venga riportati al Portafoglio                                                                            - verificare che sia stata creata la nota e sia presente la relativa icona sulla barra inferiore della polizza (accanto ai Ruoli)                                                                  </t>
+  </si>
+  <si>
+    <t>Sulla scheda della polizza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verificare che passando sull'icona della nota sia presente una tooltip che riporta la presenza di 1 nota    </t>
+  </si>
+  <si>
+    <t>Cliccando sulla nota</t>
+  </si>
+  <si>
+    <t>Verificare che:                                                                                                             - si apra la modale                                                                                                                    - sia presente il pulsante Aggiungi nota                        - sia presente il menu contestuale (tre puntini) con la possibilità di modificare o eliminare la nota</t>
+  </si>
+  <si>
+    <t>Scegliere Modifica nota</t>
+  </si>
+  <si>
+    <t>Modificare il Titolo ed il Testo.                                                                                                   - Verificare che l'operazione vada a buon fine                                                                                - Cliccando sull'icona Nota si apra la modale con il testo che ho appena modificato.</t>
+  </si>
+  <si>
+    <t>Dalla modale della nota &gt; Aggiungi nota</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inserire Titolo e Testo a piacere e cliccare su Salva                                                                   - Verificare che l'operazione vada a buon fine                                                                            - verificare che sia stata creata la nota e sia presente la relativa icona sulla barra inferiore della polizza (accanto ai Ruoli)                                                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verificare che passando sull'icona della nota sia presente una tooltip che riporta la presenza di 2 note    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inserire il Titolo e il Testo, fleggarla come Importante e cliccare su Salva                                                                   - Verificare che l'operazione vada a buon fine                                                                            - verificare che sia stata creata la nota e sia presente la relativa icona sulla barra inferiore della polizza (accanto ai Ruoli)                                                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verificare che passando sull'icona della nota sia presente una tooltip che riporta la presenza di 3 note di cui 1 importante    </t>
+  </si>
+  <si>
+    <t>Prendersi nota del numero di polizza e della Lob.                                                                  Sales &gt; Hamburger menu &gt; Note di contratto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inserire il numero di contratto, scegliere la lob &gt; Cerca                                                             - Verificare la presenza delle note                                                                                                                                             </t>
+  </si>
+  <si>
+    <t>Per una delle note, dal menu contestuale (Rotellina) &gt; Modifica</t>
+  </si>
+  <si>
+    <t>Modificare la nota &gt; scegliere Annulla                                                                             - Verificare che non sia cambiato nulla.                                                                                         .                                                                                                                                         Dal menu contestuale (Rotellina) &gt; Modifica                                                                                                               Modificare la nota &gt; scegliere Conferma                                                                                          - Verificare che l'operazione vada a buon fine ed il testo sia cambiato</t>
+  </si>
+  <si>
+    <t>In Clients sullo stesso cliente per la stessa polizza</t>
+  </si>
+  <si>
+    <t>Verificare che le modifiche siano andate a buon fine.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sempre da Clients - eliminare le note presenti </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verificare che l'operazione sia andata a buon fine </t>
+  </si>
+  <si>
+    <t>Note di contratto(1)</t>
+  </si>
+  <si>
+    <t>Note di contratto(2)</t>
+  </si>
+  <si>
+    <t>Note di contratto(3)</t>
+  </si>
+  <si>
+    <t>Note di contratto(4)</t>
+  </si>
+  <si>
+    <t>Note di contratto(5)</t>
+  </si>
+  <si>
+    <t>Note di contratto(6)</t>
+  </si>
+  <si>
+    <t>Note di contratto(7)</t>
+  </si>
+  <si>
+    <t>Note di contratto(8)</t>
+  </si>
+  <si>
+    <t>Note di contratto(9)</t>
+  </si>
+  <si>
+    <t>Note di contratto(10)</t>
+  </si>
+  <si>
+    <t>Note di contratto(11)</t>
+  </si>
+  <si>
+    <t>Note di contratto(12)</t>
+  </si>
+  <si>
+    <t>MW come delegato accedere alla scheda di un cliente con polizze AU (sia per RV/VITA/ULTRA) in vigore. Da portafoglio &gt; Menu contestuale &gt; Aggiungi nota</t>
+  </si>
+  <si>
+    <t>Matrix Web : Legami(1)</t>
+  </si>
+  <si>
+    <t>Matrix Web : Legami(2)</t>
+  </si>
+  <si>
+    <t>Matrix Web : Legami(3)</t>
+  </si>
+  <si>
+    <t>Matrix Web : Legami(4)</t>
+  </si>
+  <si>
+    <t>Matrix Web : Legami(5)</t>
+  </si>
+  <si>
+    <t>Matrix Web : Legami(6)</t>
+  </si>
+  <si>
+    <t>Matrix Web : Legami(7)</t>
+  </si>
+  <si>
+    <t>Matrix Web : Legami(8)</t>
   </si>
 </sst>
 </file>
@@ -3339,10 +3456,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10A60FA2-5DE8-44B4-9E60-8DD49A8388E4}">
-  <dimension ref="A1:I66"/>
+  <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5042,13 +5159,13 @@
     </row>
     <row r="59" spans="1:9" ht="73.5" x14ac:dyDescent="0.25">
       <c r="A59" s="20" t="s">
+        <v>292</v>
+      </c>
+      <c r="B59" s="21" t="s">
         <v>245</v>
       </c>
-      <c r="B59" s="21" t="s">
+      <c r="C59" s="21" t="s">
         <v>246</v>
-      </c>
-      <c r="C59" s="21" t="s">
-        <v>247</v>
       </c>
       <c r="D59" s="21" t="s">
         <v>130</v>
@@ -5071,13 +5188,13 @@
     </row>
     <row r="60" spans="1:9" ht="178.5" x14ac:dyDescent="0.25">
       <c r="A60" s="20" t="s">
-        <v>245</v>
+        <v>293</v>
       </c>
       <c r="B60" s="22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C60" s="21" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D60" s="21" t="s">
         <v>130</v>
@@ -5100,13 +5217,13 @@
     </row>
     <row r="61" spans="1:9" ht="42" x14ac:dyDescent="0.25">
       <c r="A61" s="20" t="s">
-        <v>251</v>
+        <v>294</v>
       </c>
       <c r="B61" s="22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C61" s="21" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D61" s="21" t="s">
         <v>130</v>
@@ -5129,13 +5246,13 @@
     </row>
     <row r="62" spans="1:9" ht="42" x14ac:dyDescent="0.25">
       <c r="A62" s="20" t="s">
-        <v>245</v>
+        <v>295</v>
       </c>
       <c r="B62" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="C62" s="21" t="s">
         <v>249</v>
-      </c>
-      <c r="C62" s="21" t="s">
-        <v>250</v>
       </c>
       <c r="D62" s="21" t="s">
         <v>130</v>
@@ -5158,13 +5275,13 @@
     </row>
     <row r="63" spans="1:9" ht="126" x14ac:dyDescent="0.25">
       <c r="A63" s="20" t="s">
-        <v>245</v>
+        <v>296</v>
       </c>
       <c r="B63" s="22" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C63" s="21" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D63" s="21" t="s">
         <v>130</v>
@@ -5187,13 +5304,13 @@
     </row>
     <row r="64" spans="1:9" ht="42" x14ac:dyDescent="0.25">
       <c r="A64" s="20" t="s">
-        <v>245</v>
+        <v>297</v>
       </c>
       <c r="B64" s="21" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C64" s="21" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D64" s="21" t="s">
         <v>130</v>
@@ -5216,13 +5333,13 @@
     </row>
     <row r="65" spans="1:9" ht="73.5" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="s">
-        <v>245</v>
+        <v>298</v>
       </c>
       <c r="B65" s="21" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C65" s="21" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D65" s="21" t="s">
         <v>130</v>
@@ -5245,13 +5362,13 @@
     </row>
     <row r="66" spans="1:9" ht="42" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
-        <v>245</v>
+        <v>299</v>
       </c>
       <c r="B66" s="21" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C66" s="21" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D66" s="21" t="s">
         <v>130</v>
@@ -5269,6 +5386,354 @@
         <v>33</v>
       </c>
       <c r="I66" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="73.5" x14ac:dyDescent="0.25">
+      <c r="A67" s="15" t="s">
+        <v>279</v>
+      </c>
+      <c r="B67" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="C67" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="D67" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="E67" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F67" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G67" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H67" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I67" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A68" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="B68" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="C68" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="D68" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="E68" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F68" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G68" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H68" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I68" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="52.5" x14ac:dyDescent="0.25">
+      <c r="A69" s="15" t="s">
+        <v>281</v>
+      </c>
+      <c r="B69" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="C69" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="D69" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="E69" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F69" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G69" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H69" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I69" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="42" x14ac:dyDescent="0.25">
+      <c r="A70" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="B70" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="C70" s="15" t="s">
+        <v>265</v>
+      </c>
+      <c r="D70" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="E70" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F70" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G70" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H70" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I70" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="A71" s="15" t="s">
+        <v>283</v>
+      </c>
+      <c r="B71" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="C71" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="D71" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="E71" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F71" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G71" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H71" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I71" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A72" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="B72" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="C72" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="D72" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="E72" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F72" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G72" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H72" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I72" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="A73" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="B73" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="C73" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="D73" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="E73" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F73" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G73" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H73" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I73" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A74" s="15" t="s">
+        <v>286</v>
+      </c>
+      <c r="B74" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="C74" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="D74" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="E74" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F74" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G74" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H74" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I74" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="42" x14ac:dyDescent="0.25">
+      <c r="A75" s="15" t="s">
+        <v>287</v>
+      </c>
+      <c r="B75" s="15" t="s">
+        <v>271</v>
+      </c>
+      <c r="C75" s="15" t="s">
+        <v>272</v>
+      </c>
+      <c r="D75" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="E75" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F75" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G75" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H75" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I75" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="73.5" x14ac:dyDescent="0.25">
+      <c r="A76" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="B76" s="15" t="s">
+        <v>273</v>
+      </c>
+      <c r="C76" s="15" t="s">
+        <v>274</v>
+      </c>
+      <c r="D76" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="E76" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F76" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G76" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H76" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I76" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A77" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="B77" s="15" t="s">
+        <v>275</v>
+      </c>
+      <c r="C77" s="15" t="s">
+        <v>276</v>
+      </c>
+      <c r="D77" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="E77" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F77" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G77" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H77" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I77" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A78" s="15" t="s">
+        <v>290</v>
+      </c>
+      <c r="B78" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="C78" s="15" t="s">
+        <v>278</v>
+      </c>
+      <c r="D78" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="E78" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F78" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G78" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H78" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I78" s="15" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>